<commit_message>
change math_model.xlsx and add module
</commit_message>
<xml_diff>
--- a/Planing/Introduction/math_model.xlsx
+++ b/Planing/Introduction/math_model.xlsx
@@ -16,13 +16,13 @@
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$10</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$11</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$B$12</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$B$13</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Sheet1!$B$15</definedName>
-    <definedName name="solver_lhs6" localSheetId="0" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="solver_lhs7" localSheetId="0" hidden="1">Sheet1!$B$17</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$15</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$16</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$B$17</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$B$18</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Sheet1!$B$18</definedName>
+    <definedName name="solver_lhs6" localSheetId="0" hidden="1">Sheet1!$B$18</definedName>
+    <definedName name="solver_lhs7" localSheetId="0" hidden="1">Sheet1!$B$18</definedName>
     <definedName name="solver_lhs8" localSheetId="0" hidden="1">Sheet1!$B$18</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
@@ -30,26 +30,26 @@
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">8</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$F$10</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel6" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel7" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs5" localSheetId="0" hidden="1">22</definedName>
-    <definedName name="solver_rhs6" localSheetId="0" hidden="1">25</definedName>
-    <definedName name="solver_rhs7" localSheetId="0" hidden="1">38</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">22</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">25</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">38</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_rhs5" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_rhs6" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_rhs7" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_rhs8" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>21 * x1 + 18 * x2 + 16 * x3 + 17,5 * x4 = f(x1, x2, x3, x4)  --&gt; max</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>период4</t>
+  </si>
+  <si>
+    <t>количество проектов претендующий на получение кредита в банке</t>
   </si>
 </sst>
 </file>
@@ -481,60 +484,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10">
-        <v>1.1034482758620692</v>
+        <v>2.4210524519575838</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
       </c>
       <c r="F10">
         <f xml:space="preserve"> 21 * B10 + 18 * B11 + 16 * B12 + 17.5 * B13</f>
-        <v>57.124437781109442</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59.263157166637065</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -542,56 +548,80 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12">
-        <v>1.3283358320839576</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.52631597972048771</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13">
-        <v>0.72563718140929534</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15">
         <f xml:space="preserve"> 8 * B10 + 7 * B11 + 5 * B12 + 9 * B13</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21.999999514263109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16">
         <f xml:space="preserve"> 8 * B10 + 9 * B11 + 7 * B12 + 8 * B13</f>
-        <v>23.931034482758619</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23.052631473704086</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17">
-        <f xml:space="preserve"> 19 * B10 + 9 * B11 + 9 * B12 + 7 * B13</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <f xml:space="preserve"> 10 * B10 + 9 * B11 + 9 * B12 + 7 * B13</f>
+        <v>28.947368337060226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="B18">
         <f xml:space="preserve"> 10 * B10 + 11 * B11 + 11 * B12 + 6 * B13</f>
-        <v>29.999999999999996</v>
+        <v>30.000000296501202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>-0.8</v>
+      </c>
+      <c r="F21" t="b">
+        <f xml:space="preserve"> 8 * D21 + 7 *D22 + 5 * D23 + 9 * D24 &lt;= 22</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>-0.98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add assignmentStatement for variable
</commit_message>
<xml_diff>
--- a/Planing/Introduction/math_model.xlsx
+++ b/Planing/Introduction/math_model.xlsx
@@ -152,7 +152,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -488,7 +488,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>